<commit_message>
Added TC13 and TC25
</commit_message>
<xml_diff>
--- a/Test_Data/Automation_Datasheet.xlsx
+++ b/Test_Data/Automation_Datasheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutmationRegression\Ecommerce_QA\Test Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutmationRegression\Ecommerce_QA\Test_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E23153-F47D-467A-8017-CE8B25331CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E528EB-45DF-4CDE-BA97-8A97F8F69834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Generic_Dataset" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="145">
   <si>
     <t>Test_Case</t>
   </si>
@@ -380,9 +380,6 @@
     <t>51051051 05105100</t>
   </si>
   <si>
-    <t>American Express</t>
-  </si>
-  <si>
     <t>3782822 46310005</t>
   </si>
   <si>
@@ -462,6 +459,15 @@
   </si>
   <si>
     <t>https://qa.checkout.wiley.com/en-gb/pdp-mock</t>
+  </si>
+  <si>
+    <t>QA_FREE1DAY_Trial_URL</t>
+  </si>
+  <si>
+    <t>https://qa.checkout.wiley.com/en-gb/cart?sku=9781119904625&amp;prom=FREE1QA</t>
+  </si>
+  <si>
+    <t>American_Express</t>
   </si>
 </sst>
 </file>
@@ -2252,10 +2258,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07745B3C-6E3C-40B5-9AC4-3C050B197A3F}">
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2315,104 +2321,104 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>140</v>
+      </c>
+      <c r="B7" s="9" t="s">
         <v>141</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>52</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>53</v>
+        <v>142</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B10" s="7" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>69</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B12" s="10" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>56</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="I13" s="9"/>
+        <v>57</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>61</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="I14" s="9"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>71</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>72</v>
+        <v>60</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>62</v>
-      </c>
-      <c r="B16" s="7">
-        <v>123</v>
+        <v>71</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>63</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
+      </c>
+      <c r="B17" s="7">
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>73</v>
-      </c>
-      <c r="B18" t="s">
-        <v>74</v>
+        <v>63</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B19" t="s">
         <v>74</v>
@@ -2420,47 +2426,47 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B20" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>78</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
+      </c>
+      <c r="B21" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>80</v>
-      </c>
-      <c r="B22" t="s">
-        <v>81</v>
+        <v>78</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>82</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>46</v>
+        <v>80</v>
+      </c>
+      <c r="B23" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>83</v>
-      </c>
-      <c r="B24" t="s">
-        <v>84</v>
+        <v>82</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B25" t="s">
         <v>84</v>
@@ -2468,138 +2474,146 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B26" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>90</v>
-      </c>
-      <c r="B28" s="7">
-        <v>222</v>
+        <v>89</v>
+      </c>
+      <c r="B28" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>96</v>
-      </c>
-      <c r="B29" t="s">
-        <v>95</v>
+        <v>90</v>
+      </c>
+      <c r="B29" s="7">
+        <v>222</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B30" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>99</v>
-      </c>
-      <c r="B31" s="7">
-        <v>11</v>
+        <v>97</v>
+      </c>
+      <c r="B31" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>100</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
+      </c>
+      <c r="B32" s="7">
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>102</v>
-      </c>
-      <c r="B33" t="s">
-        <v>103</v>
+        <v>100</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>104</v>
-      </c>
-      <c r="B34" s="7">
-        <v>12</v>
+        <v>102</v>
+      </c>
+      <c r="B34" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B35" s="7">
-        <v>49</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B36" s="7">
-        <v>0</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>107</v>
-      </c>
-      <c r="B37" t="s">
-        <v>108</v>
+        <v>106</v>
+      </c>
+      <c r="B37" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>131</v>
+        <v>107</v>
       </c>
       <c r="B38" t="s">
-        <v>132</v>
+        <v>108</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B39" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B40" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B41" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B42" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>139</v>
+      </c>
+      <c r="B43" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2607,13 +2621,14 @@
     <hyperlink ref="B2" r:id="rId1" xr:uid="{9081247E-A08E-4746-9F6C-6FD46E87BE85}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{014B7B8A-B150-4706-B7A9-1353BF798189}"/>
     <hyperlink ref="B4" r:id="rId3" xr:uid="{B8576F34-A3B1-4C25-9A3A-81A0825DD563}"/>
-    <hyperlink ref="B21" r:id="rId4" xr:uid="{DB7FC53B-5DE7-463C-B63B-0420007193A8}"/>
-    <hyperlink ref="B23" r:id="rId5" xr:uid="{248EBA86-585E-4BFB-BFF4-952F25BAABF5}"/>
+    <hyperlink ref="B22" r:id="rId4" xr:uid="{DB7FC53B-5DE7-463C-B63B-0420007193A8}"/>
+    <hyperlink ref="B24" r:id="rId5" xr:uid="{248EBA86-585E-4BFB-BFF4-952F25BAABF5}"/>
     <hyperlink ref="B5" r:id="rId6" xr:uid="{17D7A819-19DC-4D45-88DF-3C085D61A724}"/>
     <hyperlink ref="B7" r:id="rId7" xr:uid="{F7F6B453-A42E-4734-B0E6-4900FB009DF9}"/>
+    <hyperlink ref="B8" r:id="rId8" xr:uid="{749AFB31-707A-4C48-98A2-597201AA3104}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
 
@@ -2621,7 +2636,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B8EBCC8-A525-4261-B3F4-2E5AE3E9AF4C}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2679,66 +2696,66 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>144</v>
+      </c>
+      <c r="B7" t="s">
         <v>115</v>
-      </c>
-      <c r="B7" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" t="s">
         <v>117</v>
-      </c>
-      <c r="B8" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B9" t="s">
         <v>119</v>
-      </c>
-      <c r="B9" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10" t="s">
         <v>121</v>
-      </c>
-      <c r="B10" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B12" t="s">
         <v>124</v>
-      </c>
-      <c r="B12" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>125</v>
+      </c>
+      <c r="B13" t="s">
         <v>126</v>
-      </c>
-      <c r="B13" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>